<commit_message>
Completed Text Box testing
</commit_message>
<xml_diff>
--- a/src/test/java/TestData.xlsx
+++ b/src/test/java/TestData.xlsx
@@ -5,23 +5,24 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Private\Desktop\Vezba\src\test\java\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Private\Desktop\DemoQA\src\test\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E152E37C-D403-42BE-AD88-7E972D96140B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DBD171-9D79-4010-A884-7E06A6FF07FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TablePageData" sheetId="1" r:id="rId1"/>
     <sheet name="ChangedTableData" sheetId="3" r:id="rId2"/>
+    <sheet name="TextBox" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
   <si>
     <t>Firstname</t>
   </si>
@@ -60,6 +61,18 @@
   </si>
   <si>
     <t>markoivanovic@hotmail.com</t>
+  </si>
+  <si>
+    <t>currAddress</t>
+  </si>
+  <si>
+    <t>Novosadska1</t>
+  </si>
+  <si>
+    <t>permAddress</t>
+  </si>
+  <si>
+    <t>Beogradska1</t>
   </si>
 </sst>
 </file>
@@ -128,18 +141,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -358,10 +369,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="C6" sqref="A1:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -369,57 +380,53 @@
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>80600</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -431,9 +438,9 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
@@ -442,57 +449,118 @@
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+    <row r="3" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="2">
         <v>83320</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+    <row r="6" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94BE13C7-D2DD-43C0-9A68-05EFE3F8A540}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>